<commit_message>
added generated grid on parameters, and a random starting node
</commit_message>
<xml_diff>
--- a/Documents/DTT-Assessment-Hour-Log-1_updated_bonus (3).xlsx
+++ b/Documents/DTT-Assessment-Hour-Log-1_updated_bonus (3).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomr\school\bewijzenmap\periode 3.1\Stage Opdacht\DTT\DTT Assessment - Unity - 2021_\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\personal\PerfectMaze\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65381FBA-D07D-456C-89F3-9667A394FB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5DBF40-346E-44C2-A155-767D699A270C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Subject</t>
   </si>
@@ -48,25 +48,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Example 2</t>
-  </si>
-  <si>
-    <t>Had some issues with…</t>
-  </si>
-  <si>
     <t>Total amount of hours</t>
   </si>
   <si>
     <t>Bonus</t>
-  </si>
-  <si>
-    <t>Example 3</t>
-  </si>
-  <si>
-    <t>Implemented bonus feature….</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <r>
@@ -94,7 +79,13 @@
     <t>Research</t>
   </si>
   <si>
-    <t>i began with reading the assingment and beginning to do research on algorithms, i want to chose the best algoritm for a quick and customizable result</t>
+    <t>i began with reading the assingment and beginning to do research on algorithms, i want to chose the best algoritm for a quick and customizable result, i chose for randomized depth first search, because it is simple to implement without any mistakes and it will do it effectively</t>
+  </si>
+  <si>
+    <t>Implementing generation</t>
+  </si>
+  <si>
+    <t>starting with implementing the generation, also made a github, generates a grid and selects a random starting position</t>
   </si>
 </sst>
 </file>
@@ -1709,20 +1700,20 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.61328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.61328125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="6.4609375" style="1" customWidth="1"/>
-    <col min="7" max="251" width="6.4609375" customWidth="1"/>
+    <col min="1" max="1" width="24.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.59765625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
+    <col min="7" max="251" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1730,9 +1721,9 @@
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1740,7 +1731,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="24"/>
     </row>
-    <row r="3" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1754,13 +1745,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" s="17">
         <v>1</v>
@@ -1769,46 +1760,36 @@
         <v>44883</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="18">
-        <v>42736</v>
+        <v>44886</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="17">
-        <v>5</v>
-      </c>
-      <c r="C6" s="18">
-        <v>42736</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>10</v>
-      </c>
+    <row r="6" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="19"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="17"/>
       <c r="C7" s="18"/>
@@ -1816,7 +1797,7 @@
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
@@ -1824,7 +1805,7 @@
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18"/>
@@ -1832,7 +1813,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
@@ -1840,7 +1821,7 @@
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
@@ -1848,7 +1829,7 @@
       <c r="E11" s="20"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -1856,7 +1837,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
@@ -1864,7 +1845,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -1872,7 +1853,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -1880,7 +1861,7 @@
       <c r="E15" s="20"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -1888,7 +1869,7 @@
       <c r="E16" s="20"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -1896,7 +1877,7 @@
       <c r="E17" s="20"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -1904,7 +1885,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="17"/>
       <c r="C19" s="18"/>
@@ -1912,7 +1893,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -1920,7 +1901,7 @@
       <c r="E20" s="20"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -1928,7 +1909,7 @@
       <c r="E21" s="20"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="17"/>
       <c r="C22" s="18"/>
@@ -1936,7 +1917,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
@@ -1944,7 +1925,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
@@ -1952,7 +1933,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="17"/>
       <c r="C25" s="18"/>
@@ -1960,7 +1941,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
@@ -1968,7 +1949,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="17"/>
       <c r="C27" s="18"/>
@@ -1976,7 +1957,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
@@ -1984,7 +1965,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1992,20 +1973,20 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2013,7 +1994,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2021,7 +2002,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>

</xml_diff>

<commit_message>
finished maze gen/added cam movement
</commit_message>
<xml_diff>
--- a/Documents/DTT-Assessment-Hour-Log-1_updated_bonus (3).xlsx
+++ b/Documents/DTT-Assessment-Hour-Log-1_updated_bonus (3).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomr\school\bewijzenmap\periode 3.1\Stage Opdacht\PerfectMaze\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5EE295-DAD2-4FA7-9B9D-BAE2A16A5E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD9F87A-11D7-4117-BC3A-6FF069C1BDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Subject</t>
   </si>
@@ -91,7 +91,13 @@
     <t>Implementing creation</t>
   </si>
   <si>
-    <t>it now loops trough the nodes and selects one randomly that it will chose as the next node</t>
+    <t>it now loops trough the nodes and selects one randomly that it will chose as the next node and it now backtracks and removes walls (algorithm done)</t>
+  </si>
+  <si>
+    <t>Sources in the research document</t>
+  </si>
+  <si>
+    <t>implementing userstory 2</t>
   </si>
 </sst>
 </file>
@@ -1706,20 +1712,20 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.61328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.61328125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="6.4609375" style="1" customWidth="1"/>
-    <col min="7" max="251" width="6.4609375" customWidth="1"/>
+    <col min="1" max="1" width="24.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.59765625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
+    <col min="7" max="251" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1727,7 +1733,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>6</v>
       </c>
@@ -1737,7 +1743,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="24"/>
     </row>
-    <row r="3" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1755,7 +1761,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1771,12 +1777,12 @@
       <c r="E4" s="20"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="18">
         <v>44886</v>
@@ -1787,12 +1793,12 @@
       <c r="E5" s="20"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="18">
         <v>44889</v>
@@ -1803,15 +1809,19 @@
       <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+    <row r="7" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
+      <c r="C7" s="18">
+        <v>44892</v>
+      </c>
       <c r="D7" s="15"/>
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
@@ -1819,7 +1829,7 @@
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18"/>
@@ -1827,7 +1837,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
@@ -1835,7 +1845,7 @@
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
@@ -1843,7 +1853,7 @@
       <c r="E11" s="20"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -1851,7 +1861,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
@@ -1859,7 +1869,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -1867,7 +1877,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -1875,7 +1885,7 @@
       <c r="E15" s="20"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -1883,7 +1893,7 @@
       <c r="E16" s="20"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -1891,7 +1901,7 @@
       <c r="E17" s="20"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -1899,7 +1909,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="17"/>
       <c r="C19" s="18"/>
@@ -1907,7 +1917,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -1915,7 +1925,7 @@
       <c r="E20" s="20"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -1923,7 +1933,7 @@
       <c r="E21" s="20"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="17"/>
       <c r="C22" s="18"/>
@@ -1931,7 +1941,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
@@ -1939,7 +1949,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
@@ -1947,7 +1957,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="17"/>
       <c r="C25" s="18"/>
@@ -1955,7 +1965,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
@@ -1963,7 +1973,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="17"/>
       <c r="C27" s="18"/>
@@ -1971,15 +1981,17 @@
       <c r="E27" s="20"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
+    <row r="28" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
       <c r="D28" s="15"/>
       <c r="E28" s="20"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1987,20 +1999,20 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2008,7 +2020,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2016,7 +2028,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>

</xml_diff>